<commit_message>
añadido csv con el idioma.
</commit_message>
<xml_diff>
--- a/src/main/resources/misc/objetos y equipamiento.xlsx
+++ b/src/main/resources/misc/objetos y equipamiento.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gDrivePer\workspaces\java\IntelliJWS\BeginningOfTime\src\main\resources\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAC0E581-2B9B-4FC7-9CE1-607E48A31BA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7554C6F9-6B85-4294-B164-5297B6A695E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="objetos" sheetId="1" r:id="rId1"/>
     <sheet name="equipamiento" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">equipamiento!$A$1:$H$16</definedName>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="276">
   <si>
     <t>ID</t>
   </si>
@@ -241,13 +242,637 @@
   </si>
   <si>
     <t>40 ar 40 mr 70 agl</t>
+  </si>
+  <si>
+    <t>ESPAÑOL</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>Idea original: Shiku.</t>
+  </si>
+  <si>
+    <t>Programador: Shiku.</t>
+  </si>
+  <si>
+    <t>Diseños conceptuales: Josert</t>
+  </si>
+  <si>
+    <t>Testers: Dakos, Josert.</t>
+  </si>
+  <si>
+    <t>Traductor al ingles: Dakos.</t>
+  </si>
+  <si>
+    <t>Historia basada en el origen de tiid.</t>
+  </si>
+  <si>
+    <t>Empezar de nuevo</t>
+  </si>
+  <si>
+    <t>Nueva Partida</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
+    <t>Historial de cambios</t>
+  </si>
+  <si>
+    <t>Cambiar Idioma (Change Language)</t>
+  </si>
+  <si>
+    <t>Salir del juego</t>
+  </si>
+  <si>
+    <t>ITEMS UPDATE 0.5 (ACTUAL)</t>
+  </si>
+  <si>
+    <t>Juego publicado en GitHub!</t>
+  </si>
+  <si>
+    <t>Posibilidad de empezar Nueva Partida +, con tus personajes de la anterior partida y enemigos mas complicados.</t>
+  </si>
+  <si>
+    <t>Ahora los enemigos se dividen en 4 tipos.</t>
+  </si>
+  <si>
+    <t>Rama de habilidades de apoyo sustituidas por objetos.</t>
+  </si>
+  <si>
+    <t>Estadisticas rediseñadas por completo, con mas niveles.</t>
+  </si>
+  <si>
+    <t>Añadido nuevos menus, para incrementar la accesibilidad.</t>
+  </si>
+  <si>
+    <t>Ahora para subir de nivel sera necesario alcanzar cierto nivel de XP.</t>
+  </si>
+  <si>
+    <t>Ahora cada personaje tiene inventario propio, con posibilidad de usar objetos y equiparse armadura.</t>
+  </si>
+  <si>
+    <t>Revisadas todas las opciones y mejorada la seleccion de las mismas.</t>
+  </si>
+  <si>
+    <t>Añadida posibilidad de que los enemigos suelten objetos, equipamiento y experiencia despues de cada combate.</t>
+  </si>
+  <si>
+    <t>Añadida historia.</t>
+  </si>
+  <si>
+    <t>Nombre cambiado a The Beginning of Time.</t>
+  </si>
+  <si>
+    <t>CONTENT UPDATE 0.6 (PROXIMAMENTE)</t>
+  </si>
+  <si>
+    <t>Traduccion a otros idiomas.</t>
+  </si>
+  <si>
+    <t>Mas enemigos, personajes, objetos y equipamiento.</t>
+  </si>
+  <si>
+    <t>Fisico</t>
+  </si>
+  <si>
+    <t>Magico</t>
+  </si>
+  <si>
+    <t>Varios</t>
+  </si>
+  <si>
+    <t>Bloquear</t>
+  </si>
+  <si>
+    <t>Inventario</t>
+  </si>
+  <si>
+    <t>Volver</t>
+  </si>
+  <si>
+    <t>Barrido</t>
+  </si>
+  <si>
+    <t>Gran Golpe</t>
+  </si>
+  <si>
+    <t>Ataque rapido</t>
+  </si>
+  <si>
+    <t>Marginado</t>
+  </si>
+  <si>
+    <t>Mago</t>
+  </si>
+  <si>
+    <t>Caballero</t>
+  </si>
+  <si>
+    <t>Asesino</t>
+  </si>
+  <si>
+    <t>Tanque</t>
+  </si>
+  <si>
+    <t>AquaSplash</t>
+  </si>
+  <si>
+    <t>Combustion</t>
+  </si>
+  <si>
+    <t>Tornado</t>
+  </si>
+  <si>
+    <t>Estadisticas de Personajes y Enemigos</t>
+  </si>
+  <si>
+    <t>Informacion del Juego</t>
+  </si>
+  <si>
+    <t>Informacion de los ataques</t>
+  </si>
+  <si>
+    <t>AYUDA SOBRE LAS CLASES</t>
+  </si>
+  <si>
+    <t>Sera capaz de aguantar mas golpes que ninguna clase, pero sera poco agil.</t>
+  </si>
+  <si>
+    <t>Nivel 20: (HP: 320, AD: 3, AP: 6, AR: 13, MR: 13, AGL: 4)</t>
+  </si>
+  <si>
+    <t>Tendra mas posibilidad de esquivar los ataques, pero a cambio tendra muy poca armadura.</t>
+  </si>
+  <si>
+    <t>Nivel 20: (HP: 200,  AD: 18, AP: 4, AR: 5, MR: 5, AGL: 18)</t>
+  </si>
+  <si>
+    <t>Esta clase hara un daño normal, y recibira daño normal.</t>
+  </si>
+  <si>
+    <t>Nivel 20: (HP: 250,  AD: 12, AP: 7, AR: 8, MR: 8, AGL: 10)</t>
+  </si>
+  <si>
+    <t>Clase para jugadores veteranos. Sera capaz de realizar mucho daño, pero tendra muy poca resistencia.</t>
+  </si>
+  <si>
+    <t>Nivel 20: (HP: 160,  AD: 5, AP: 20, AR: 6, MR: 10, AGL: 12)</t>
+  </si>
+  <si>
+    <t>y sus estadisticas no aumentaran tanto como las otras clases. Un verdadero reto.</t>
+  </si>
+  <si>
+    <t>Nivel 20: (HP: 180,  AD: 8, AP: 8, AR: 5, MR: 6, AGL: 6)</t>
+  </si>
+  <si>
+    <t>Tanque: Clase especializada en la resistencia y el aguante. Mucha vida y armadura.</t>
+  </si>
+  <si>
+    <t>Asesino: Clase especializada en el daño Fisico. Mucho daño fisico y agilidad.</t>
+  </si>
+  <si>
+    <t>Caballero: Clase especializada en la estabilidad. Tendra un poco de todo.</t>
+  </si>
+  <si>
+    <t>Mago: Clase especializada en el daño Magico. Mucho daño magico.</t>
+  </si>
+  <si>
+    <t>Marginado: Clase para jugadores curtidos. No tiene ninguna ventaja. Le costara mas subir de nivel,</t>
+  </si>
+  <si>
+    <t>Aqui ira la ayuda del juego.</t>
+  </si>
+  <si>
+    <t>Aqui ira la historia del juego.</t>
+  </si>
+  <si>
+    <t>changelogMenu0</t>
+  </si>
+  <si>
+    <t>changelogMenu1</t>
+  </si>
+  <si>
+    <t>changelogMenu2</t>
+  </si>
+  <si>
+    <t>changelogMenu3</t>
+  </si>
+  <si>
+    <t>changelogMenu4</t>
+  </si>
+  <si>
+    <t>changelogMenu5</t>
+  </si>
+  <si>
+    <t>changelogMenu6</t>
+  </si>
+  <si>
+    <t>changelogMenu7</t>
+  </si>
+  <si>
+    <t>changelogMenu8</t>
+  </si>
+  <si>
+    <t>changelogMenu9</t>
+  </si>
+  <si>
+    <t>changelogMenu10</t>
+  </si>
+  <si>
+    <t>changelogMenu11</t>
+  </si>
+  <si>
+    <t>changelogMenu12</t>
+  </si>
+  <si>
+    <t>changelogMenu13</t>
+  </si>
+  <si>
+    <t>changelogMenu14</t>
+  </si>
+  <si>
+    <t>changelogMenu15</t>
+  </si>
+  <si>
+    <t>extras0</t>
+  </si>
+  <si>
+    <t>extras1</t>
+  </si>
+  <si>
+    <t>extras2</t>
+  </si>
+  <si>
+    <t>extras3</t>
+  </si>
+  <si>
+    <t>extras4</t>
+  </si>
+  <si>
+    <t>extras5</t>
+  </si>
+  <si>
+    <t>class0</t>
+  </si>
+  <si>
+    <t>class1</t>
+  </si>
+  <si>
+    <t>class2</t>
+  </si>
+  <si>
+    <t>class3</t>
+  </si>
+  <si>
+    <t>class4</t>
+  </si>
+  <si>
+    <t>attack0</t>
+  </si>
+  <si>
+    <t>attack1</t>
+  </si>
+  <si>
+    <t>attack2</t>
+  </si>
+  <si>
+    <t>attack3</t>
+  </si>
+  <si>
+    <t>attack4</t>
+  </si>
+  <si>
+    <t>attack5</t>
+  </si>
+  <si>
+    <t>Ayuda e informacion sobre las clases.</t>
+  </si>
+  <si>
+    <t>option0</t>
+  </si>
+  <si>
+    <t>classInfo0</t>
+  </si>
+  <si>
+    <t>classInfo1</t>
+  </si>
+  <si>
+    <t>classInfo2</t>
+  </si>
+  <si>
+    <t>classInfo3</t>
+  </si>
+  <si>
+    <t>classInfo4</t>
+  </si>
+  <si>
+    <t>classInfo5</t>
+  </si>
+  <si>
+    <t>classInfo6</t>
+  </si>
+  <si>
+    <t>classInfo7</t>
+  </si>
+  <si>
+    <t>classInfo8</t>
+  </si>
+  <si>
+    <t>classInfo9</t>
+  </si>
+  <si>
+    <t>classInfo10</t>
+  </si>
+  <si>
+    <t>classInfo11</t>
+  </si>
+  <si>
+    <t>classInfo12</t>
+  </si>
+  <si>
+    <t>classInfo13</t>
+  </si>
+  <si>
+    <t>classInfo14</t>
+  </si>
+  <si>
+    <t>classInfo15</t>
+  </si>
+  <si>
+    <t>gameInfo0</t>
+  </si>
+  <si>
+    <t>gameStory0</t>
+  </si>
+  <si>
+    <t>message1</t>
+  </si>
+  <si>
+    <t>option1</t>
+  </si>
+  <si>
+    <t>option2</t>
+  </si>
+  <si>
+    <t>option3</t>
+  </si>
+  <si>
+    <t>option4</t>
+  </si>
+  <si>
+    <t>option5</t>
+  </si>
+  <si>
+    <t>option6</t>
+  </si>
+  <si>
+    <t>option7</t>
+  </si>
+  <si>
+    <t>option8</t>
+  </si>
+  <si>
+    <t>option9</t>
+  </si>
+  <si>
+    <t>option10</t>
+  </si>
+  <si>
+    <t>option11</t>
+  </si>
+  <si>
+    <t>option12</t>
+  </si>
+  <si>
+    <t>option13</t>
+  </si>
+  <si>
+    <t>option14</t>
+  </si>
+  <si>
+    <t>option15</t>
+  </si>
+  <si>
+    <t>message2</t>
+  </si>
+  <si>
+    <t>message3</t>
+  </si>
+  <si>
+    <t>message4</t>
+  </si>
+  <si>
+    <t>message5</t>
+  </si>
+  <si>
+    <t>message6</t>
+  </si>
+  <si>
+    <t>message7</t>
+  </si>
+  <si>
+    <t>message8</t>
+  </si>
+  <si>
+    <t>message9</t>
+  </si>
+  <si>
+    <t>message10</t>
+  </si>
+  <si>
+    <t>message11</t>
+  </si>
+  <si>
+    <t>message12</t>
+  </si>
+  <si>
+    <t>message13</t>
+  </si>
+  <si>
+    <t>message14</t>
+  </si>
+  <si>
+    <t>message15</t>
+  </si>
+  <si>
+    <t>message16</t>
+  </si>
+  <si>
+    <t>message17</t>
+  </si>
+  <si>
+    <t>message18</t>
+  </si>
+  <si>
+    <t>message19</t>
+  </si>
+  <si>
+    <t>message20</t>
+  </si>
+  <si>
+    <t>message21</t>
+  </si>
+  <si>
+    <t>message22</t>
+  </si>
+  <si>
+    <t>message23</t>
+  </si>
+  <si>
+    <t>message24</t>
+  </si>
+  <si>
+    <t>message25</t>
+  </si>
+  <si>
+    <t>message26</t>
+  </si>
+  <si>
+    <t>message27</t>
+  </si>
+  <si>
+    <t>message28</t>
+  </si>
+  <si>
+    <t>Que quieres hacer?</t>
+  </si>
+  <si>
+    <t>Como quieres llamar al personaje?</t>
+  </si>
+  <si>
+    <t>Bienvenido a The Beginning of Time!</t>
+  </si>
+  <si>
+    <t>Turno de</t>
+  </si>
+  <si>
+    <t>Comienza el juego</t>
+  </si>
+  <si>
+    <t>ha sido creado.</t>
+  </si>
+  <si>
+    <t>ha subido al nivel</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>Hasta la proxima!</t>
+  </si>
+  <si>
+    <t>Que clase quieres elegir?</t>
+  </si>
+  <si>
+    <t>Estas Seguro? (1:si/2:no)</t>
+  </si>
+  <si>
+    <t>Pulsa enter para continuar....</t>
+  </si>
+  <si>
+    <t>Has derrotado a todos los Enemigos!</t>
+  </si>
+  <si>
+    <t>Todos los personajes han muerto. Has perdido.</t>
+  </si>
+  <si>
+    <t>Que enemigo quieres elegir?</t>
+  </si>
+  <si>
+    <t>El enemigo que has elegido esta muerto.</t>
+  </si>
+  <si>
+    <t>Bloquear pasara el turno y reducira el daño del siguiente ataque recibido.</t>
+  </si>
+  <si>
+    <t>Quieres bloquear?</t>
+  </si>
+  <si>
+    <t>Vacio</t>
+  </si>
+  <si>
+    <t>Elige una clase para tu Personaje:</t>
+  </si>
+  <si>
+    <t>El enemigo ha esquivado el ataque!</t>
+  </si>
+  <si>
+    <t>errorMessage0</t>
+  </si>
+  <si>
+    <t>El Enemigo especificado no ha sido encontrado.</t>
+  </si>
+  <si>
+    <t>El Personaje especificado no ha sido encontrado.</t>
+  </si>
+  <si>
+    <t>Introduce un numero valido.</t>
+  </si>
+  <si>
+    <t>El ataque seleccionado no esta disponible.</t>
+  </si>
+  <si>
+    <t>El juego ha encontrado un error y debe cerrarse.</t>
+  </si>
+  <si>
+    <t>Bloquear ya estaba activo.</t>
+  </si>
+  <si>
+    <t>Ahora</t>
+  </si>
+  <si>
+    <t>esta bloqueando.</t>
+  </si>
+  <si>
+    <t>Introduce un nombre valido.</t>
+  </si>
+  <si>
+    <t>errorMessage1</t>
+  </si>
+  <si>
+    <t>errorMessage2</t>
+  </si>
+  <si>
+    <t>errorMessage3</t>
+  </si>
+  <si>
+    <t>errorMessage4</t>
+  </si>
+  <si>
+    <t>errorMessage5</t>
+  </si>
+  <si>
+    <t>errorMessage6</t>
+  </si>
+  <si>
+    <t>Gracias por jugar!</t>
+  </si>
+  <si>
+    <t>El enemigo estaba bloqueando.</t>
+  </si>
+  <si>
+    <t>Ataque critico!</t>
+  </si>
+  <si>
+    <t>Has conseguido realizar</t>
+  </si>
+  <si>
+    <t>pts de daño.</t>
+  </si>
+  <si>
+    <t>ha muerto.</t>
+  </si>
+  <si>
+    <t>message29</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +899,12 @@
       <b/>
       <sz val="8"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -317,12 +948,21 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -333,7 +973,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -375,6 +1015,11 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Énfasis1" xfId="1" builtinId="30"/>
@@ -661,7 +1306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
@@ -1245,4 +1890,862 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CA1E5F6-DBC4-4BBD-882A-3F5832EBB4F6}">
+  <dimension ref="A1:C104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="106.140625" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="17" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>195</v>
+      </c>
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>196</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>197</v>
+      </c>
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>198</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>199</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>200</v>
+      </c>
+      <c r="B13" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>201</v>
+      </c>
+      <c r="B14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>202</v>
+      </c>
+      <c r="B15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>203</v>
+      </c>
+      <c r="B16" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="B17" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>139</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>140</v>
+      </c>
+      <c r="B22" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>141</v>
+      </c>
+      <c r="B23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>143</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>144</v>
+      </c>
+      <c r="B26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>145</v>
+      </c>
+      <c r="B27" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>147</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>148</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>150</v>
+      </c>
+      <c r="B32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B33" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>152</v>
+      </c>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>153</v>
+      </c>
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>155</v>
+      </c>
+      <c r="B37" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>156</v>
+      </c>
+      <c r="B38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>158</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>159</v>
+      </c>
+      <c r="B41" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>160</v>
+      </c>
+      <c r="B42" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>163</v>
+      </c>
+      <c r="B45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>164</v>
+      </c>
+      <c r="B46" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>165</v>
+      </c>
+      <c r="B47" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>166</v>
+      </c>
+      <c r="B48" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>167</v>
+      </c>
+      <c r="B49" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="B50" s="15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>171</v>
+      </c>
+      <c r="B51" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>173</v>
+      </c>
+      <c r="B53" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>174</v>
+      </c>
+      <c r="B54" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>176</v>
+      </c>
+      <c r="B56" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>177</v>
+      </c>
+      <c r="B57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>178</v>
+      </c>
+      <c r="B58" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>180</v>
+      </c>
+      <c r="B60" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>181</v>
+      </c>
+      <c r="B61" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>182</v>
+      </c>
+      <c r="B62" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>183</v>
+      </c>
+      <c r="B63" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>185</v>
+      </c>
+      <c r="B65" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="B66" s="15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>187</v>
+      </c>
+      <c r="B67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>189</v>
+      </c>
+      <c r="B69" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>205</v>
+      </c>
+      <c r="B70" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>206</v>
+      </c>
+      <c r="B71" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>207</v>
+      </c>
+      <c r="B72" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>208</v>
+      </c>
+      <c r="B73" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>209</v>
+      </c>
+      <c r="B74" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>210</v>
+      </c>
+      <c r="B75" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>211</v>
+      </c>
+      <c r="B76" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>212</v>
+      </c>
+      <c r="B77" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>213</v>
+      </c>
+      <c r="B78" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>214</v>
+      </c>
+      <c r="B79" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>215</v>
+      </c>
+      <c r="B80" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>216</v>
+      </c>
+      <c r="B81" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>217</v>
+      </c>
+      <c r="B82" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>218</v>
+      </c>
+      <c r="B83" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>219</v>
+      </c>
+      <c r="B84" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>220</v>
+      </c>
+      <c r="B85" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>221</v>
+      </c>
+      <c r="B86" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>222</v>
+      </c>
+      <c r="B87" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>223</v>
+      </c>
+      <c r="B88" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>224</v>
+      </c>
+      <c r="B89" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>225</v>
+      </c>
+      <c r="B90" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>226</v>
+      </c>
+      <c r="B91" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="B92" s="16" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="B93" s="18" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A94" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="B94" s="18" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
+        <v>230</v>
+      </c>
+      <c r="B95" s="18" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="16" t="s">
+        <v>231</v>
+      </c>
+      <c r="B96" s="18" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="15" t="s">
+        <v>275</v>
+      </c>
+      <c r="B97" s="19" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>253</v>
+      </c>
+      <c r="B98" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>263</v>
+      </c>
+      <c r="B99" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>264</v>
+      </c>
+      <c r="B100" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>265</v>
+      </c>
+      <c r="B101" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>266</v>
+      </c>
+      <c r="B102" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>267</v>
+      </c>
+      <c r="B103" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" s="15" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="15" t="s">
+        <v>268</v>
+      </c>
+      <c r="B104" s="15" t="s">
+        <v>262</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>